<commit_message>
add efrontier.py & max_sharpe_portfolio func
</commit_message>
<xml_diff>
--- a/investments.xlsx
+++ b/investments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.eff_fron_spyder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_A9E65DD621076E1A42C3EAFABDB7E11B12967B63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E28ED4D-C7F9-4A6E-9A88-AD9155023D52}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="11_A9E65DD621076E1A42C3EAFABDB7E11B12967B63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DDA2040-BA36-4052-9097-4C6515F2801B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,20 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="CASH" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -36,10 +49,13 @@
     <t>Ticker</t>
   </si>
   <si>
-    <t>Min Weight (%)</t>
+    <t>Min Weight</t>
   </si>
   <si>
-    <t>Max Weight (%)</t>
+    <t>Max Weight</t>
+  </si>
+  <si>
+    <t>BIL</t>
   </si>
   <si>
     <t>AGG</t>
@@ -57,7 +73,7 @@
     <t>IVV</t>
   </si>
   <si>
-    <t>IWN</t>
+    <t>IWM</t>
   </si>
   <si>
     <t>EFA</t>
@@ -67,9 +83,6 @@
   </si>
   <si>
     <t>IYR</t>
-  </si>
-  <si>
-    <t>BIL</t>
   </si>
 </sst>
 </file>
@@ -144,20 +157,20 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -174,6 +187,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -467,32 +484,32 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="11">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7">
         <v>0</v>
       </c>
       <c r="C2" s="7">
@@ -501,9 +518,9 @@
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="11">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7">
         <v>0</v>
       </c>
       <c r="C3" s="7">
@@ -512,9 +529,9 @@
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="11">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7">
         <v>0</v>
       </c>
       <c r="C4" s="7">
@@ -523,9 +540,9 @@
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="11">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7">
         <v>0</v>
       </c>
       <c r="C5" s="7">
@@ -534,9 +551,9 @@
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="11">
+        <v>10</v>
+      </c>
+      <c r="B6" s="7">
         <v>0</v>
       </c>
       <c r="C6" s="7">
@@ -545,9 +562,9 @@
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="11">
+        <v>11</v>
+      </c>
+      <c r="B7" s="7">
         <v>0</v>
       </c>
       <c r="C7" s="7">
@@ -555,21 +572,21 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="11">
+      <c r="A8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="7">
         <v>0</v>
       </c>
       <c r="C8" s="7">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="11">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7">
         <v>0</v>
       </c>
       <c r="C9" s="7">
@@ -578,9 +595,9 @@
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="11">
+        <v>14</v>
+      </c>
+      <c r="B10" s="7">
         <v>0</v>
       </c>
       <c r="C10" s="7">
@@ -589,9 +606,9 @@
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="11">
+        <v>15</v>
+      </c>
+      <c r="B11" s="7">
         <v>0</v>
       </c>
       <c r="C11" s="7">

</xml_diff>